<commit_message>
Add Darwin plot & add Darwin to Combined
</commit_message>
<xml_diff>
--- a/EUC_Perth_Assets.xlsx
+++ b/EUC_Perth_Assets.xlsx
@@ -267,7 +267,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C118"/>
+  <dimension ref="A1:C120"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
@@ -2281,6 +2281,40 @@
       <c r="C118" t="inlineStr">
         <is>
           <t>2024-03-10 15:26:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>SAN125998</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>2024-11-17 13:16:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>SAN125999</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>2024-11-17 13:16:47</t>
         </is>
       </c>
     </row>
@@ -2399,6 +2433,12 @@
           <t xml:space="preserve">Laptop Charger </t>
         </is>
       </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="inlineStr">
@@ -2413,6 +2453,12 @@
           <t xml:space="preserve">Monitor 24” </t>
         </is>
       </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="inlineStr">
@@ -2420,6 +2466,12 @@
           <t>Monitor 34” Ultrawide</t>
         </is>
       </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="inlineStr">
@@ -2427,6 +2479,12 @@
           <t>USB DVD-RW Drive</t>
         </is>
       </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="inlineStr">
@@ -2440,6 +2498,12 @@
         <is>
           <t>Wired Keyboard</t>
         </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="16">
@@ -2474,7 +2538,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:XFD1"/>
@@ -2522,7 +2586,6 @@
           <t>add 25</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2540,7 +2603,6 @@
           <t>add 10</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2558,7 +2620,96 @@
           <t>subtract 1</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-11-17 13:20:05</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Laptop Charger </t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>add 30</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-11-17 13:20:08</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monitor 24” </t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>add 30</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-11-17 13:20:09</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Monitor 34” Ultrawide</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>add 30</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-11-17 13:20:11</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>USB DVD-RW Drive</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>add 30</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-11-17 13:20:12</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Wired Keyboard</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>add 30</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2979,10 +3130,10 @@
         </is>
       </c>
       <c r="B2" s="1" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
@@ -3213,7 +3364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1" sqref="A1:XFD1"/>
@@ -3763,9 +3914,67 @@
         </is>
       </c>
     </row>
-    <row r="28" ht="12.75" customHeight="1"/>
-    <row r="29" ht="12.75" customHeight="1"/>
-    <row r="30" ht="12.75" customHeight="1"/>
+    <row r="28" ht="12.75" customHeight="1">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-11-17 13:16:43</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>SAN125998</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" ht="12.75" customHeight="1">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-11-17 13:16:47</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>SAN125999</t>
+        </is>
+      </c>
+    </row>
+    <row r="30" ht="12.75" customHeight="1">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-11-17 13:16:47</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>add 2</t>
+        </is>
+      </c>
+    </row>
     <row r="31" ht="12.75" customHeight="1"/>
     <row r="32" ht="12.75" customHeight="1"/>
     <row r="33" ht="12.75" customHeight="1"/>
@@ -4131,8 +4340,12 @@
           <t xml:space="preserve">Laptop Charger </t>
         </is>
       </c>
-      <c r="B9" s="1" t="n"/>
-      <c r="C9" s="1" t="n"/>
+      <c r="B9" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="4" t="inlineStr">
@@ -4260,7 +4473,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:F1048576"/>
@@ -4672,8 +4885,42 @@
         </is>
       </c>
     </row>
-    <row r="20" ht="12.75" customHeight="1"/>
-    <row r="21" ht="12.75" customHeight="1"/>
+    <row r="20" ht="12.75" customHeight="1">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-11-17 13:19:45</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Laptop Charger </t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>add 5</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
+    </row>
+    <row r="21" ht="12.75" customHeight="1">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-11-17 13:19:57</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Laptop Charger </t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>add 30</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr"/>
+    </row>
     <row r="22" ht="12.75" customHeight="1"/>
     <row r="23" ht="12.75" customHeight="1"/>
     <row r="24" ht="12.75" customHeight="1"/>
@@ -4736,6 +4983,12 @@
           <t>Laptop 840 G6</t>
         </is>
       </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
@@ -4743,12 +4996,24 @@
           <t xml:space="preserve">Monitor 24” </t>
         </is>
       </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="inlineStr">
         <is>
           <t>Monitor 34” Ultrawide</t>
         </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="5">
@@ -4804,7 +5069,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A4"/>
@@ -4839,8 +5104,59 @@
       <c r="E1" s="2" t="n"/>
       <c r="F1" s="2" t="n"/>
     </row>
-    <row r="2" ht="17.25" customHeight="1"/>
-    <row r="4" ht="15" customHeight="1"/>
+    <row r="2" ht="17.25" customHeight="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2024-11-17 12:22:50</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monitor 24” </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>add 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-11-17 13:20:29</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Monitor 34” Ultrawide</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>add 30</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-11-17 13:20:35</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Laptop 840 G6</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>add 15</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4952,7 +5268,6 @@
           <t>add 2</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add Location data to "All_SANs", "SANs in Stock"
</commit_message>
<xml_diff>
--- a/EUC_Perth_Assets.xlsx
+++ b/EUC_Perth_Assets.xlsx
@@ -267,7 +267,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C120"/>
+  <dimension ref="A1:D123"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
@@ -294,6 +294,11 @@
           <t>Time</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="1" t="inlineStr">
@@ -2315,6 +2320,62 @@
       <c r="C120" t="inlineStr">
         <is>
           <t>2024-11-17 13:16:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>SAN126998</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>2024-11-17 14:54:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>SAN126999</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>2024-11-17 14:54:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>SAN126985</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>2024-11-17 14:56:48</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Darwin</t>
         </is>
       </c>
     </row>
@@ -2372,6 +2433,12 @@
           <t>Desktop Mini G9</t>
         </is>
       </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
@@ -2405,6 +2472,12 @@
         <is>
           <t>Laptop 840 G10</t>
         </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -2538,7 +2611,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:XFD1"/>
@@ -2637,7 +2710,6 @@
           <t>add 30</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2655,7 +2727,6 @@
           <t>add 30</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2673,7 +2744,6 @@
           <t>add 30</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2691,7 +2761,6 @@
           <t>add 30</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2709,7 +2778,168 @@
           <t>add 30</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-11-17 14:54:43</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>SAN126998</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-11-17 14:54:47</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>SAN126999</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-11-17 14:54:47</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>add 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-11-17 14:56:43</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>SAN126987</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-11-17 14:56:48</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>SAN126985</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-11-17 14:56:49</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>add 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-11-17 14:58:12</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>subtract</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>SAN126987</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-11-17 14:58:12</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>subtract 1</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4901,7 +5131,6 @@
           <t>add 5</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" t="inlineStr">
@@ -4919,7 +5148,6 @@
           <t>add 30</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
     </row>
     <row r="22" ht="12.75" customHeight="1"/>
     <row r="23" ht="12.75" customHeight="1"/>
@@ -5137,7 +5365,6 @@
           <t>add 30</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4" ht="15" customHeight="1">
       <c r="A4" t="inlineStr">
@@ -5155,7 +5382,6 @@
           <t>add 15</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Layout remains the same but focus on improving usability for entering multiple SANs.
</commit_message>
<xml_diff>
--- a/EUC_Perth_Assets.xlsx
+++ b/EUC_Perth_Assets.xlsx
@@ -267,7 +267,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D131"/>
+  <dimension ref="A1:D143"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
@@ -2552,6 +2552,270 @@
       <c r="D131" t="inlineStr">
         <is>
           <t>Darwin</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>SAN444444</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:44:41</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>BR</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>SAN343435</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:49:44</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>BR</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>SAN555444</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:49:46</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>BR</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>SAN45453</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:49:54</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>BR</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>SAN456753</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:52:31</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>SAN111567</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:52:32</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>SAN494946</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:52:37</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>SAN166544</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:52:40</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>SAN493574</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:56:13</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>SAN165478</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:56:16</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>SAN254687</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:56:18</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>SAN264578</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:56:19</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>4.2</t>
         </is>
       </c>
     </row>
@@ -2703,10 +2967,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C11" t="n">
-        <v>30</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12">
@@ -2760,6 +3024,12 @@
         <is>
           <t>Wired Mouse</t>
         </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="17">
@@ -2793,7 +3063,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:XFD1"/>
@@ -3348,7 +3618,40 @@
           <t>add 4</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:42:55</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monitor 24” </t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>add 24</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:43:00</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Wired Mouse</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>add 24</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3873,10 +4176,10 @@
         </is>
       </c>
       <c r="B10" s="1" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1">
@@ -4003,7 +4306,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1" sqref="A1:XFD1"/>
@@ -4647,18 +4950,218 @@
           <t>subtract 2</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr"/>
-    </row>
-    <row r="33" ht="12.75" customHeight="1"/>
-    <row r="34" ht="12.75" customHeight="1"/>
-    <row r="35" ht="12.75" customHeight="1"/>
-    <row r="36" ht="12.75" customHeight="1"/>
-    <row r="37" ht="12.75" customHeight="1"/>
-    <row r="38" ht="12.75" customHeight="1"/>
-    <row r="39" ht="12.75" customHeight="1"/>
-    <row r="40" ht="12.75" customHeight="1"/>
-    <row r="41" ht="12.75" customHeight="1"/>
-    <row r="42" ht="12.75" customHeight="1"/>
+    </row>
+    <row r="33" ht="12.75" customHeight="1">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:52:31</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>SAN456753</t>
+        </is>
+      </c>
+    </row>
+    <row r="34" ht="12.75" customHeight="1">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:52:32</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>SAN111567</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" ht="12.75" customHeight="1">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:52:37</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>SAN494946</t>
+        </is>
+      </c>
+    </row>
+    <row r="36" ht="12.75" customHeight="1">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:52:40</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>SAN166544</t>
+        </is>
+      </c>
+    </row>
+    <row r="37" ht="12.75" customHeight="1">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:52:40</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>add 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="38" ht="12.75" customHeight="1">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:56:13</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>SAN493574</t>
+        </is>
+      </c>
+    </row>
+    <row r="39" ht="12.75" customHeight="1">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:56:16</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>SAN165478</t>
+        </is>
+      </c>
+    </row>
+    <row r="40" ht="12.75" customHeight="1">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:56:18</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>SAN254687</t>
+        </is>
+      </c>
+    </row>
+    <row r="41" ht="12.75" customHeight="1">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:56:19</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>SAN264578</t>
+        </is>
+      </c>
+    </row>
+    <row r="42" ht="12.75" customHeight="1">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:56:20</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>add 4</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr"/>
+    </row>
     <row r="43" ht="12.75" customHeight="1"/>
     <row r="44" ht="12.75" customHeight="1"/>
     <row r="45" ht="12.75" customHeight="1"/>
@@ -4981,8 +5484,12 @@
           <t>Laptop 840 G10</t>
         </is>
       </c>
-      <c r="B6" s="1" t="n"/>
-      <c r="C6" s="1" t="n"/>
+      <c r="B6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" s="4" t="inlineStr">
@@ -5145,7 +5652,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:F1048576"/>
@@ -5591,11 +6098,128 @@
         </is>
       </c>
     </row>
-    <row r="22" ht="12.75" customHeight="1"/>
-    <row r="23" ht="12.75" customHeight="1"/>
-    <row r="24" ht="12.75" customHeight="1"/>
-    <row r="25" ht="12.75" customHeight="1"/>
-    <row r="26" ht="12.75" customHeight="1"/>
+    <row r="22" ht="12.75" customHeight="1">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:44:41</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>SAN444444</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" ht="12.75" customHeight="1">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:44:41</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="12.75" customHeight="1">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:49:44</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>SAN343435</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="12.75" customHeight="1">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:49:46</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>SAN555444</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" ht="12.75" customHeight="1">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:49:54</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>SAN45453</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:49:54</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>add 3</t>
+        </is>
+      </c>
+    </row>
     <row r="1048576" ht="12.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -5654,10 +6278,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C2" t="n">
-        <v>15</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3">
@@ -5667,10 +6291,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4">
@@ -5739,7 +6363,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A4"/>
@@ -5839,6 +6463,40 @@
       <c r="C5" t="inlineStr">
         <is>
           <t>subtract 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:43:11</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monitor 24” </t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>add 24</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:43:14</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Laptop 840 G6</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>add 24</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Search function in "All SANs" list
</commit_message>
<xml_diff>
--- a/EUC_Perth_Assets.xlsx
+++ b/EUC_Perth_Assets.xlsx
@@ -267,7 +267,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D143"/>
+  <dimension ref="A1:D146"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
@@ -2816,6 +2816,72 @@
       <c r="D143" t="inlineStr">
         <is>
           <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>SAN482659</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>2024-11-17 19:03:41</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Darwin</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>SAN356784</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>2024-11-17 19:03:43</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Darwin</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>SAN154687</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>2024-11-17 19:03:45</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Darwin</t>
         </is>
       </c>
     </row>
@@ -2959,6 +3025,12 @@
           <t>Laptop x360 G8</t>
         </is>
       </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="inlineStr">
@@ -3063,7 +3135,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:XFD1"/>
@@ -3652,6 +3724,90 @@
           <t>add 24</t>
         </is>
       </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-11-17 19:03:41</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>SAN482659</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-11-17 19:03:43</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>SAN356784</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-11-17 19:03:45</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>SAN154687</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-11-17 19:03:45</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>add 3</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4098,10 +4254,10 @@
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
@@ -4306,7 +4462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1" sqref="A1:XFD1"/>
@@ -5160,9 +5316,24 @@
           <t>add 4</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr"/>
-    </row>
-    <row r="43" ht="12.75" customHeight="1"/>
+    </row>
+    <row r="43" ht="12.75" customHeight="1">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2024-11-17 18:59:55</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt G2</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>add 6</t>
+        </is>
+      </c>
+    </row>
     <row r="44" ht="12.75" customHeight="1"/>
     <row r="45" ht="12.75" customHeight="1"/>
     <row r="46" ht="12.75" customHeight="1"/>

</xml_diff>

<commit_message>
Add "Bold" button text when selected
</commit_message>
<xml_diff>
--- a/EUC_Perth_Assets.xlsx
+++ b/EUC_Perth_Assets.xlsx
@@ -267,7 +267,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D146"/>
+  <dimension ref="A1:D149"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
@@ -2882,6 +2882,72 @@
       <c r="D146" t="inlineStr">
         <is>
           <t>Darwin</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>SAN457865</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>2024-11-17 20:05:59</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>SAN125335</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>2024-11-17 23:27:40</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>SAN125448</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>2024-11-17 23:27:42</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>4.2</t>
         </is>
       </c>
     </row>
@@ -3807,7 +3873,6 @@
           <t>add 3</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4280,10 +4345,10 @@
         </is>
       </c>
       <c r="B6" s="1" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
@@ -4462,7 +4527,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1" sqref="A1:XFD1"/>
@@ -5334,11 +5399,106 @@
         </is>
       </c>
     </row>
-    <row r="44" ht="12.75" customHeight="1"/>
-    <row r="45" ht="12.75" customHeight="1"/>
-    <row r="46" ht="12.75" customHeight="1"/>
-    <row r="47" ht="12.75" customHeight="1"/>
-    <row r="48" ht="12.75" customHeight="1"/>
+    <row r="44" ht="12.75" customHeight="1">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2024-11-17 20:05:59</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>SAN457865</t>
+        </is>
+      </c>
+    </row>
+    <row r="45" ht="12.75" customHeight="1">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2024-11-17 20:05:59</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="46" ht="12.75" customHeight="1">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2024-11-17 23:27:40</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>SAN125335</t>
+        </is>
+      </c>
+    </row>
+    <row r="47" ht="12.75" customHeight="1">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2024-11-17 23:27:42</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>SAN125448</t>
+        </is>
+      </c>
+    </row>
+    <row r="48" ht="12.75" customHeight="1">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2024-11-17 23:27:43</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>add 2</t>
+        </is>
+      </c>
+    </row>
     <row r="49" ht="12.75" customHeight="1"/>
     <row r="50" ht="12.75" customHeight="1"/>
     <row r="51" ht="12.75" customHeight="1"/>
@@ -6714,10 +6874,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -6731,7 +6891,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -6783,6 +6943,24 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-11-17 23:48:42</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Laptop 840 G6</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>add 2</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve plot functionality, ease of use
</commit_message>
<xml_diff>
--- a/EUC_Perth_Assets.xlsx
+++ b/EUC_Perth_Assets.xlsx
@@ -274,7 +274,7 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="25.42578125" customWidth="1" style="1" min="1" max="3"/>
   </cols>
@@ -2978,7 +2978,7 @@
       <selection activeCell="A1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="28" customWidth="1" min="1" max="1"/>
   </cols>
@@ -3892,7 +3892,7 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.42578125" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="12.5703125" customWidth="1" min="2" max="2"/>
     <col width="11.5703125" customWidth="1" min="16384" max="16384"/>
@@ -4490,7 +4490,7 @@
       <selection activeCell="A1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="28" customWidth="1" min="1" max="1"/>
   </cols>
@@ -4558,10 +4558,10 @@
         </is>
       </c>
       <c r="B5" s="1" t="n">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
@@ -4753,13 +4753,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="18.42578125" customWidth="1" min="1" max="1"/>
     <col width="20.5703125" customWidth="1" min="2" max="2"/>
@@ -5759,7 +5759,24 @@
         </is>
       </c>
     </row>
-    <row r="51" ht="12.75" customHeight="1"/>
+    <row r="51" ht="12.75" customHeight="1">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2024-11-19 23:10:18</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt G4</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>subtract 3</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr"/>
+    </row>
     <row r="52" ht="12" customHeight="1"/>
     <row r="53" ht="12" customHeight="1"/>
     <row r="54" ht="12" customHeight="1"/>
@@ -6001,7 +6018,7 @@
       <selection activeCell="A6" activeCellId="2" sqref="A11 A12 A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="28" customWidth="1" min="1" max="1"/>
   </cols>
@@ -6247,7 +6264,7 @@
       <selection activeCell="E1" sqref="E1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="18.5703125" customWidth="1" min="1" max="1"/>
     <col width="17.140625" customWidth="1" min="2" max="2"/>
@@ -6836,7 +6853,7 @@
       <selection activeCell="A1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="28" customWidth="1" min="1" max="1"/>
     <col width="10" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -6958,7 +6975,7 @@
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="20.85546875" customWidth="1" min="1" max="1"/>
   </cols>

</xml_diff>